<commit_message>
Update ToDO and Bug list
</commit_message>
<xml_diff>
--- a/items/ToDo_Bug_List.xlsx
+++ b/items/ToDo_Bug_List.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yijing/Documents/Document/080.ANU/10.Courses/09.COMP6442/03.Ass/02.GroupProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yijing/StudioProjects/ga-23s2/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2264C4A-97DE-5248-A705-C125DF574150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF63DB9-7B92-F146-96E3-C34AB8E0A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="840" windowWidth="27640" windowHeight="16940" xr2:uid="{708D4608-1F1E-C948-A177-CA1AB144B87D}"/>
   </bookViews>
   <sheets>
     <sheet name="ToDO_Bug" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>输入检索关键词后，直接进入case detail页面，而不是检索结果页</t>
+  </si>
+  <si>
+    <t>首页的scam case列表添加下拉刷新功能</t>
+  </si>
+  <si>
+    <t>在添加post之后下拉列表刷新，主页显示新添加的案例</t>
+  </si>
+  <si>
+    <t>Profile添加修改照片和名字的功能</t>
+  </si>
+  <si>
+    <t>点击头像，能够上传图片，点击名字可以修改</t>
+  </si>
+  <si>
+    <t>重构firebaseauth和firestore的代码，形成单例模式和state模式</t>
+  </si>
+  <si>
+    <t>相关所有功能正常运行</t>
+  </si>
+  <si>
+    <t>Zhaoyun</t>
+  </si>
+  <si>
+    <t>用户读取数据和添加数据加入权限</t>
   </si>
 </sst>
 </file>
@@ -154,12 +178,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -479,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DA20EA-845A-AC4D-9D55-7ADD0DCC2F57}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -517,8 +538,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <f>ROW()-1</f>
+      <c r="A2" s="1">
+        <f t="shared" ref="A2:A7" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -527,7 +548,7 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -538,11 +559,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <f>ROW()-1</f>
+      <c r="A3" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -553,8 +574,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <f>ROW()-1</f>
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -574,8 +595,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <f>ROW()-1</f>
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D5" t="s">
@@ -589,8 +610,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <f>ROW()-1</f>
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -610,8 +631,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <f>ROW()-1</f>
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D7" t="s">
@@ -625,8 +646,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <f t="shared" ref="A8:A16" si="0">ROW()-1</f>
+      <c r="A8" s="1">
+        <f t="shared" ref="A8:A16" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -646,8 +667,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <f t="shared" si="0"/>
+      <c r="A9" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -667,8 +688,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <f t="shared" si="0"/>
+      <c r="A10" s="1">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -688,8 +709,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <f t="shared" si="0"/>
+      <c r="A11" s="1">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -703,8 +724,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
+      <c r="A12" s="1">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -718,27 +739,89 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <f t="shared" si="0"/>
+      <c r="A13" s="1">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>13</v>
+      <c r="A14" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
+      <c r="A15" s="1">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
+      <c r="A16" s="1">
+        <f t="shared" si="1"/>
         <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>